<commit_message>
commit as intermediate backup
</commit_message>
<xml_diff>
--- a/mapping_summary.xlsx
+++ b/mapping_summary.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,37 +442,32 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Match_string</t>
+          <t>original</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Match_string_modified</t>
+          <t>modified</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Match_string__tidied</t>
+          <t>tidied</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Exact</t>
+          <t>match</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>ASCII</t>
+          <t>alias</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Regex</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Fuzzy</t>
+          <t>method</t>
         </is>
       </c>
     </row>
@@ -500,10 +495,13 @@
           <t>sampling date</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>sampling date</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -529,10 +527,13 @@
           <t>locationid</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>locationid</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -558,10 +559,13 @@
           <t>sampleid</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>sampleid</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -589,18 +593,17 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
+          <t>Phosphate</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>PO4</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>PO4</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>PO4</t>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>exact</t>
         </is>
       </c>
     </row>
@@ -630,18 +633,17 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>Phosphate</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>PO4</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>PO4</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>PO4</t>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>exact</t>
         </is>
       </c>
     </row>
@@ -669,12 +671,19 @@
           <t>nitrate</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr">
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>nitrate</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>NO3</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>fuzzy</t>
         </is>
       </c>
     </row>
@@ -702,12 +711,19 @@
           <t>nitrate</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr">
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nitrate</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>NO3</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>fuzzy</t>
         </is>
       </c>
     </row>
@@ -735,10 +751,13 @@
           <t>nitrite</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nitrite</t>
+        </is>
+      </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -764,10 +783,13 @@
           <t>nitrite</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nitrite</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -793,10 +815,13 @@
           <t>ammonium</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>ammonium</t>
+        </is>
+      </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -822,10 +847,13 @@
           <t>ammonium</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>ammonium</t>
+        </is>
+      </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -851,10 +879,13 @@
           <t>silica</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>silica</t>
+        </is>
+      </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -880,10 +911,13 @@
           <t>silica</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>silica</t>
+        </is>
+      </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -911,18 +945,17 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
+          <t>Sulphate</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>SO4</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>SO4</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>SO4</t>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>exact</t>
         </is>
       </c>
     </row>
@@ -952,18 +985,17 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
+          <t>Sulphate</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
           <t>SO4</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>SO4</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>SO4</t>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>exact</t>
         </is>
       </c>
     </row>
@@ -991,10 +1023,13 @@
           <t>sodium</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>sodium</t>
+        </is>
+      </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1020,10 +1055,13 @@
           <t xml:space="preserve"> 18</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 18</t>
+        </is>
+      </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1049,10 +1087,13 @@
           <t>calcium</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>calcium</t>
+        </is>
+      </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1078,10 +1119,13 @@
           <t>calcium</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>calcium</t>
+        </is>
+      </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1107,10 +1151,13 @@
           <t>it worked</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>it worked</t>
+        </is>
+      </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1136,16 +1183,19 @@
           <t>atpinhibition</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>atpinhibition</t>
+        </is>
+      </c>
       <c r="G22" t="inlineStr">
         <is>
           <t>TEST</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>TEST</t>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>ascii</t>
         </is>
       </c>
     </row>
@@ -1173,10 +1223,13 @@
           <t>arsenic</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>arsenic</t>
+        </is>
+      </c>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1202,10 +1255,13 @@
           <t>arsenic</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>arsenic</t>
+        </is>
+      </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1231,10 +1287,13 @@
           <t>acidity</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>acidity</t>
+        </is>
+      </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1260,10 +1319,13 @@
           <t>acidity</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>acidity</t>
+        </is>
+      </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1289,10 +1351,13 @@
           <t>electrical conductivity</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>electrical conductivity</t>
+        </is>
+      </c>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1318,10 +1383,13 @@
           <t>ec</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr"/>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>ec</t>
+        </is>
+      </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1347,14 +1415,13 @@
           <t>ecoli</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr"/>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>ecoli</t>
+        </is>
+      </c>
       <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>E.coli</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1380,14 +1447,13 @@
           <t>ecoli</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr"/>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>ecoli</t>
+        </is>
+      </c>
       <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>E.coli</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1413,10 +1479,13 @@
           <t>it worked</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr"/>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>it worked</t>
+        </is>
+      </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1442,10 +1511,13 @@
           <t>sample number</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr"/>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>sample number</t>
+        </is>
+      </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1458,7 +1530,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1474,17 +1546,27 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Match_string</t>
+          <t>original</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Match_string_modified</t>
+          <t>modified</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Regex</t>
+          <t>match</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>alias</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>method</t>
         </is>
       </c>
     </row>
@@ -1500,6 +1582,12 @@
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -1513,6 +1601,12 @@
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -1526,6 +1620,12 @@
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -1551,6 +1651,16 @@
           <t>mg/l</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>mg / (1l)</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -1576,6 +1686,16 @@
           <t>mg P/l</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>mg / (1l)</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1601,6 +1721,16 @@
           <t>mg/l</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>mg / (1l)</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1626,6 +1756,16 @@
           <t>ug N/l</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>ug / (1l)</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1651,6 +1791,16 @@
           <t>mmol/l</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>mmol / (1l)</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1676,6 +1826,16 @@
           <t>umol N/l</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>umol / (1l)</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1701,6 +1861,16 @@
           <t>mg/l</t>
         </is>
       </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>mg / (1l)</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1726,6 +1896,16 @@
           <t>mg N/l</t>
         </is>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>mg / (1l)</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1751,6 +1931,16 @@
           <t>mg/l</t>
         </is>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>mg / (1l)</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1776,6 +1966,16 @@
           <t>mg Si/l</t>
         </is>
       </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>mg / (1l)</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1801,6 +2001,16 @@
           <t>mg/l</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>mg / (1l)</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1826,6 +2036,16 @@
           <t>mg S/l</t>
         </is>
       </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>mg / (1l)</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1851,6 +2071,16 @@
           <t>mg/l</t>
         </is>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>mg / (1l)</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1864,6 +2094,12 @@
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1889,6 +2125,16 @@
           <t>mg/l</t>
         </is>
       </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>mg / (1l)</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1914,6 +2160,16 @@
           <t>ug/l</t>
         </is>
       </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>ug / (1l)</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1934,7 +2190,17 @@
           <t>wrong</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>wrong</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1955,7 +2221,13 @@
           <t>%</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1981,6 +2253,16 @@
           <t>ug/l</t>
         </is>
       </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>ug / (1l)</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -2006,6 +2288,16 @@
           <t>ug/l</t>
         </is>
       </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>ug / (1l)</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -2026,7 +2318,17 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="E25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -2047,7 +2349,13 @@
           <t>wrong_unit</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr"/>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>wrong_unit</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -2073,6 +2381,16 @@
           <t>uS/cm</t>
         </is>
       </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>uS / (1cm)</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -2098,6 +2416,16 @@
           <t>mS/m</t>
         </is>
       </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>mS / (1m)</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -2118,7 +2446,21 @@
           <t>n/100mL</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr"/>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>n/100mL</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>n / (100mL)</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -2144,6 +2486,16 @@
           <t>kve/L</t>
         </is>
       </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>kve / (1L)</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -2157,6 +2509,12 @@
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -2170,6 +2528,12 @@
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>regex</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>